<commit_message>
Updated BOM and added M2.5 screws
</commit_message>
<xml_diff>
--- a/Components/Enabled_Controller_BOM.xlsx
+++ b/Components/Enabled_Controller_BOM.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milad\Development\Enabled-Controller\Components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\Enabled-Controller\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79191736-8B63-4E79-B1E0-515E77AB84AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C10C55D-9613-4271-AF6E-BF0E1101FB8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Enabled-Controller" sheetId="1" r:id="rId1"/>
+    <sheet name="Enabled_Controller_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Index</t>
   </si>
@@ -115,6 +115,25 @@
   <si>
     <t xml:space="preserve">	
 1528-2500-ND</t>
+  </si>
+  <si>
+    <t>36-4701-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+HEX NUT 0.245" STEEL 6-32</t>
+  </si>
+  <si>
+    <t>36-9309-ND</t>
+  </si>
+  <si>
+    <t>MACH SCREW PAN HEAD SLOTTED 6-32</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/keystone-electronics/4701/316272</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/keystone-electronics/9309/2746088</t>
   </si>
 </sst>
 </file>
@@ -174,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,15 +208,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,18 +535,18 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D10:D11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.89453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.3671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="2" customWidth="1"/>
     <col min="3" max="4" width="24" style="2" customWidth="1"/>
     <col min="5" max="5" width="32" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.62890625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.5234375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.89453125" style="2"/>
+    <col min="6" max="6" width="16.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -565,7 +584,7 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2">
@@ -698,25 +717,55 @@
       <c r="I6"/>
       <c r="J6"/>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="H7" s="4"/>
+    <row r="7" spans="1:10" ht="28.8">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4701</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="I7"/>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10">
+        <v>9309</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I8"/>
       <c r="J8"/>
     </row>
@@ -754,7 +803,7 @@
       </c>
       <c r="G11">
         <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8+F9*B9</f>
-        <v>38.17</v>
+        <v>38.769999999999996</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -796,8 +845,10 @@
     <hyperlink ref="H4" r:id="rId2" xr:uid="{7F734AD5-2ECA-40F7-A5CE-C5DEF5C93822}"/>
     <hyperlink ref="H5" r:id="rId3" xr:uid="{701E6E80-BE8A-4941-A46E-83BDD619D55E}"/>
     <hyperlink ref="H2" r:id="rId4" xr:uid="{56B0595D-98AE-4748-9AC9-C718094D26A8}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{2FFF1290-1E84-4F07-99B8-567479417876}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{52359737-FFB5-4289-8BA5-9CE4DDD30DB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM for two versions
</commit_message>
<xml_diff>
--- a/Components/Enabled_Controller_BOM.xlsx
+++ b/Components/Enabled_Controller_BOM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\Enabled-Controller\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C10C55D-9613-4271-AF6E-BF0E1101FB8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B3CA67-FD3D-491A-9B4F-520F7AA1BEA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Enabled_Controller_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="USB Enabled_Controller_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Wireless Enabled_Controller_BOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Index</t>
   </si>
@@ -105,16 +106,6 @@
   </si>
   <si>
     <t>CP-43514-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/3675/1528-2500-ND/8031669</t>
-  </si>
-  <si>
-    <t>ITSY BITSY 32U4 3V 8MHZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	
-1528-2500-ND</t>
   </si>
   <si>
     <t>36-4701-ND</t>
@@ -134,6 +125,24 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/keystone-electronics/9309/2746088</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adafruit-industries-llc/3727/8346575</t>
+  </si>
+  <si>
+    <t>1528-2554-ND</t>
+  </si>
+  <si>
+    <t>ITSYBITSY M0 EXPRESS ATSAMD21</t>
+  </si>
+  <si>
+    <t>1528-4481-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	ITSYBITSY NRF52840 EXPRESS BLE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adafruit-industries-llc/4481/11497502</t>
   </si>
 </sst>
 </file>
@@ -534,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -577,7 +586,7 @@
       <c r="I1"/>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:10" ht="28.8">
+    <row r="2" spans="1:10">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -585,22 +594,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2">
-        <v>3675</v>
+        <v>3727</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2">
-        <v>14.35</v>
+        <v>16.91</v>
       </c>
       <c r="G2" s="2">
-        <v>14.35</v>
+        <v>16.91</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -725,20 +734,22 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="10">
         <v>4701</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" s="10">
         <v>0.15</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="10">
+        <v>0.15</v>
+      </c>
       <c r="H7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -751,20 +762,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="10">
         <v>9309</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="10">
         <v>0.15</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="10">
+        <v>0.15</v>
+      </c>
       <c r="H8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -802,8 +815,8 @@
         <v>14</v>
       </c>
       <c r="G11">
-        <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8+F9*B9</f>
-        <v>38.769999999999996</v>
+        <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8</f>
+        <v>41.33</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -851,4 +864,262 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AC8FF3-46C8-4A12-BB0E-916354D8384F}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4481</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2">
+        <v>25.4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>25.4</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.26</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.37</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.37</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.72</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.72</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>1.53</v>
+      </c>
+      <c r="G6">
+        <v>1.53</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4701</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="10">
+        <v>9309</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8</f>
+        <v>49.819999999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{874A0235-A94B-4A5D-B717-0C7C0A768758}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{44311824-40A1-4F32-B4FC-D783F9568938}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{8D26BADF-F9D3-4FC1-8341-96FA65754CC0}"/>
+    <hyperlink ref="H2" r:id="rId4" xr:uid="{782923B7-E322-46D3-8C0F-79F4B37DFE70}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{091A55B0-BEDD-443C-9426-62E17713C38A}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{714F5C83-35A8-4E20-885A-F4C28C8DBD90}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM file : Price updated and changed screw part
</commit_message>
<xml_diff>
--- a/Components/Enabled_Controller_BOM.xlsx
+++ b/Components/Enabled_Controller_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\Enabled-Controller\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B3CA67-FD3D-491A-9B4F-520F7AA1BEA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDF18FD-132D-413F-861B-961C27C2D271}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>S7047-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">	PPPC141LFBN-RC</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/PPPC141LFBN-RC/S7047-ND/810186</t>
   </si>
   <si>
@@ -111,10 +108,6 @@
     <t>36-4701-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">	
-HEX NUT 0.245" STEEL 6-32</t>
-  </si>
-  <si>
     <t>36-9309-ND</t>
   </si>
   <si>
@@ -143,6 +136,12 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/adafruit-industries-llc/4481/11497502</t>
+  </si>
+  <si>
+    <t>HEX NUT 0.245" STEEL 6-32</t>
+  </si>
+  <si>
+    <t>PPPC141LFBN-RC</t>
   </si>
 </sst>
 </file>
@@ -544,7 +543,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="A1:H11"/>
+      <selection activeCell="G8" sqref="F3:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -594,22 +593,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2">
         <v>3727</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F2" s="2">
-        <v>16.91</v>
+        <v>16.54</v>
       </c>
       <c r="G2" s="2">
-        <v>16.91</v>
+        <v>16.54</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -631,13 +630,14 @@
         <v>5</v>
       </c>
       <c r="F3" s="2">
-        <v>4.26</v>
+        <v>4.08</v>
       </c>
       <c r="G3" s="2">
-        <v>0.85199999999999998</v>
+        <f>F3/5</f>
+        <v>0.81600000000000006</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -653,19 +653,19 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="2">
-        <v>1.37</v>
+        <v>1.32</v>
       </c>
       <c r="G4" s="2">
-        <v>1.37</v>
+        <v>1.32</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -687,10 +687,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="2">
-        <v>1.72</v>
+        <v>1.65</v>
       </c>
       <c r="G5" s="2">
-        <v>1.72</v>
+        <v>1.65</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>12</v>
@@ -706,27 +706,27 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="G6">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
     </row>
-    <row r="7" spans="1:10" ht="28.8">
+    <row r="7" spans="1:10">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -734,13 +734,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10">
         <v>4701</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F7" s="10">
         <v>0.15</v>
@@ -749,7 +749,7 @@
         <v>0.15</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -762,13 +762,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="10">
         <v>9309</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="10">
         <v>0.15</v>
@@ -777,7 +777,7 @@
         <v>0.15</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -816,7 +816,7 @@
       </c>
       <c r="G11">
         <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8</f>
-        <v>41.33</v>
+        <v>39.999999999999986</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -860,9 +860,10 @@
     <hyperlink ref="H2" r:id="rId4" xr:uid="{56B0595D-98AE-4748-9AC9-C718094D26A8}"/>
     <hyperlink ref="H7" r:id="rId5" xr:uid="{2FFF1290-1E84-4F07-99B8-567479417876}"/>
     <hyperlink ref="H8" r:id="rId6" xr:uid="{52359737-FFB5-4289-8BA5-9CE4DDD30DB4}"/>
+    <hyperlink ref="H6" r:id="rId7" xr:uid="{30F97266-541A-4C4E-9218-D9A255AD989F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -871,7 +872,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -918,13 +919,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2">
         <v>4481</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" s="2">
         <v>25.4</v>
@@ -933,7 +934,7 @@
         <v>25.4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -953,13 +954,14 @@
         <v>5</v>
       </c>
       <c r="F3" s="2">
-        <v>4.26</v>
+        <v>4.08</v>
       </c>
       <c r="G3" s="2">
-        <v>0.85199999999999998</v>
+        <f>F3/5</f>
+        <v>0.81600000000000006</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -973,19 +975,19 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="2">
-        <v>1.37</v>
+        <v>1.32</v>
       </c>
       <c r="G4" s="2">
-        <v>1.37</v>
+        <v>1.32</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1005,10 +1007,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="2">
-        <v>1.72</v>
+        <v>1.65</v>
       </c>
       <c r="G5" s="2">
-        <v>1.72</v>
+        <v>1.65</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>12</v>
@@ -1022,25 +1024,25 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="G6">
-        <v>1.53</v>
+        <v>1.47</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1048,13 +1050,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10">
         <v>4701</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F7" s="10">
         <v>0.15</v>
@@ -1063,7 +1065,7 @@
         <v>0.15</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1074,13 +1076,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="10">
         <v>9309</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="10">
         <v>0.15</v>
@@ -1089,7 +1091,7 @@
         <v>0.15</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1108,7 +1110,7 @@
       </c>
       <c r="G11">
         <f>F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8</f>
-        <v>49.819999999999993</v>
+        <v>48.859999999999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>